<commit_message>
Updated to include IU field server in totals
</commit_message>
<xml_diff>
--- a/CReSIS Data Volumes.xlsx
+++ b/CReSIS Data Volumes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\scripts\archive_ct_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\scripts\ct_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14085" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Year Total" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1514,11 +1513,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R365"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B328" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B356" sqref="B356"/>
+      <selection pane="bottomRight" activeCell="M112" sqref="M112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,8 +4181,8 @@
         <v/>
       </c>
       <c r="M113" s="5">
-        <f>SUM(K114:K150,K32:K34,K55:K69,K71,K224:K227,K52:K53,K325:K328)</f>
-        <v>632.28893222194165</v>
+        <f>SUM(K114:K150,K32:K34,K55:K69,K71,K224:K227,K52:K53,K325:K328,K336)</f>
+        <v>637.78893222194165</v>
       </c>
       <c r="N113" s="5">
         <f>SUM(L114:L150,L32:L34,L55:L69,L71,L224:L227,L52:L53)</f>
@@ -4191,7 +4190,7 @@
       </c>
       <c r="O113" s="5">
         <f>M113+N113</f>
-        <v>786.77353111356501</v>
+        <v>792.27353111356501</v>
       </c>
       <c r="P113" s="4" t="s">
         <v>308</v>
@@ -7769,8 +7768,8 @@
         <v/>
       </c>
       <c r="M268" s="5">
-        <f>SUM(K269:K293,K330:K332)</f>
-        <v>194.97716698888689</v>
+        <f>SUM(K269:K293,K330:K332,K338)</f>
+        <v>205.97716698888689</v>
       </c>
       <c r="N268" s="5">
         <f>SUM(L269:L293)</f>
@@ -7778,7 +7777,7 @@
       </c>
       <c r="O268" s="5">
         <f>M268+N268</f>
-        <v>204.59575756080449</v>
+        <v>215.59575756080449</v>
       </c>
       <c r="P268" s="4" t="s">
         <v>311</v>
@@ -7861,7 +7860,7 @@
         <v>2317662019</v>
       </c>
       <c r="C272">
-        <f t="shared" ref="C272:C324" si="17">B272/(1024*1024*1024)</f>
+        <f t="shared" ref="C272:C319" si="17">B272/(1024*1024*1024)</f>
         <v>2.1584909586235881</v>
       </c>
       <c r="H272" s="10">
@@ -9589,8 +9588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9675,7 +9674,7 @@
       </c>
       <c r="B6" s="11">
         <f>Individual!M113</f>
-        <v>632.28893222194165</v>
+        <v>637.78893222194165</v>
       </c>
       <c r="C6" s="11">
         <f>Individual!N113</f>
@@ -9683,7 +9682,7 @@
       </c>
       <c r="D6" s="11">
         <f>Individual!O113</f>
-        <v>786.77353111356501</v>
+        <v>792.27353111356501</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -9692,7 +9691,7 @@
       </c>
       <c r="B7" s="11">
         <f>Individual!M268</f>
-        <v>194.97716698888689</v>
+        <v>205.97716698888689</v>
       </c>
       <c r="C7" s="11">
         <f>Individual!N268</f>
@@ -9700,7 +9699,7 @@
       </c>
       <c r="D7" s="11">
         <f>Individual!O268</f>
-        <v>204.59575756080449</v>
+        <v>215.59575756080449</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -9709,7 +9708,7 @@
       </c>
       <c r="B8" s="12">
         <f>SUM(B3:B7)</f>
-        <v>1023.3945206953213</v>
+        <v>1039.8945206953213</v>
       </c>
       <c r="C8" s="12">
         <f>SUM(C3:C7)</f>
@@ -9717,7 +9716,7 @@
       </c>
       <c r="D8" s="12">
         <f>SUM(D3:D7)</f>
-        <v>1210.9302275460213</v>
+        <v>1227.4302275460213</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -9726,11 +9725,11 @@
       </c>
       <c r="B9" s="13">
         <f>B8/$D8</f>
-        <v>0.84513087328677428</v>
+        <v>0.84721273548425091</v>
       </c>
       <c r="C9" s="13">
         <f>C8/$D8</f>
-        <v>0.15486912671322575</v>
+        <v>0.15278726451574912</v>
       </c>
       <c r="D9" s="13">
         <f>D8/$D8</f>

</xml_diff>